<commit_message>
Agent step completed: Update divisions page with data alignment fix and new features
</commit_message>
<xml_diff>
--- a/0-UFCnextChamp-Sheet.xlsx
+++ b/0-UFCnextChamp-Sheet.xlsx
@@ -578,7 +578,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1993-07-12 00:00:00</t>
+          <t>07/12/1993</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -600,11 +600,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Mexico</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -624,11 +620,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -648,11 +640,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -672,11 +660,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -696,11 +680,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Muay Thai</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -720,11 +700,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -744,11 +720,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -768,11 +740,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -792,11 +760,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -816,11 +780,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -840,11 +800,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -864,11 +820,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -888,11 +840,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -912,11 +860,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1049,11 +993,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sugar</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -1073,11 +1013,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>24/10/1994</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -1097,11 +1033,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -1121,11 +1053,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -1145,11 +1073,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -1169,11 +1093,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Kickboxing</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -1193,11 +1113,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -1217,11 +1133,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1241,11 +1153,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -1265,11 +1173,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -1289,11 +1193,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1313,11 +1213,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -1337,11 +1233,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1361,11 +1253,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -1385,11 +1273,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1409,11 +1293,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1546,11 +1426,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>The Great</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -1570,11 +1446,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>29/09/1988</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -1594,11 +1466,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -1618,11 +1486,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -1642,11 +1506,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Lucha Libre Olímpica (Wrestling)</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -1666,11 +1526,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -1690,11 +1546,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -1714,11 +1566,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1738,11 +1586,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -1762,11 +1606,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -1786,11 +1626,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1810,11 +1646,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -1834,11 +1666,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1858,11 +1686,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -1882,11 +1706,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1906,11 +1726,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2043,11 +1859,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -2067,11 +1879,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>27/10/1991</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -2091,11 +1899,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -2115,11 +1919,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -2139,11 +1939,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Sambo</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -2163,11 +1959,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -2187,11 +1979,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Lucha Libre Olímpica (Wrestling)</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -2211,11 +1999,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -2235,11 +2019,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -2259,11 +2039,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -2283,11 +2059,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -2307,11 +2079,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -2331,11 +2099,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -2355,11 +2119,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -2379,11 +2139,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -2403,11 +2159,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2540,11 +2292,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Rocky</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -2564,11 +2312,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>25/08/1991</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -2588,11 +2332,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -2612,11 +2352,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Jamaica</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -2636,11 +2372,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -2660,11 +2392,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -2684,11 +2412,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Lucha Libre Olímpica (Wrestling)</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -2708,11 +2432,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -2732,11 +2452,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -2756,11 +2472,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -2780,11 +2492,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -2804,11 +2512,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -2828,11 +2532,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -2852,11 +2552,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -2876,11 +2572,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -2900,11 +2592,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3037,11 +2725,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Tarzan</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -3061,11 +2745,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>27/02/1991</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -3085,11 +2765,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -3109,11 +2785,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -3133,11 +2805,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -3157,11 +2825,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -3181,11 +2845,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Lucha Libre Olímpica (Wrestling)</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -3205,11 +2865,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -3229,11 +2885,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -3253,11 +2905,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -3277,11 +2925,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -3301,11 +2945,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -3325,11 +2965,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -3349,11 +2985,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -3373,11 +3005,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3397,11 +3025,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3534,11 +3158,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Poatan</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -3558,11 +3178,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>07/07/1987</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -3582,11 +3198,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -3606,11 +3218,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -3630,11 +3238,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Kickboxing</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -3654,11 +3258,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -3678,11 +3278,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -3702,11 +3298,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -3726,11 +3318,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -3750,11 +3338,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -3774,11 +3358,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -3798,11 +3378,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -3822,11 +3398,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -3846,11 +3418,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -3870,11 +3438,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -3894,11 +3458,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4031,11 +3591,7 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Bones</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -4055,11 +3611,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>19/07/1987</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -4079,11 +3631,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -4103,11 +3651,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -4127,11 +3671,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Lucha Libre Olímpica (Wrestling)</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -4151,11 +3691,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Jiu-Jitsu Brasileño (BJJ)</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -4175,11 +3711,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Muay Thai</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -4199,11 +3731,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -4223,11 +3751,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -4247,11 +3771,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -4271,11 +3791,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -4295,11 +3811,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -4319,11 +3831,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -4343,11 +3851,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
     </row>
@@ -4367,11 +3871,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -4391,11 +3891,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>